<commit_message>
modified:   build/log_in/Analysis-00.toc 	modified:   build/log_in/EXE-00.toc 	modified:   build/log_in/PKG-00.toc 	modified:   build/log_in/PYZ-00.pyz 	modified:   build/log_in/PYZ-00.toc 	modified:   build/log_in/Tree-00.toc 	modified:   build/log_in/Tree-01.toc 	modified:   build/log_in/Tree-02.toc 	modified:   build/log_in/base_library.zip 	modified:   build/log_in/log_in.pkg 	modified:   build/log_in/warn-log_in.txt 	modified:   build/log_in/xref-log_in.html 	modified:   database/mybd 	modified:   interfaces/analista_calidad/show_analyst_data.ui 	renamed:    dist/log_in.exe -> log_in.exe 	deleted:    log_in.spec 	modified:   media/docs/BLANCO.xlsx 	modified:   source/__pycache__/conection.cpython-312.pyc 	modified:   source/__pycache__/cuestionario.cpython-312.pyc 	modified:   source/conection.py 	modified:   source/showAnalystData.py
</commit_message>
<xml_diff>
--- a/media/docs/BLANCO.xlsx
+++ b/media/docs/BLANCO.xlsx
@@ -8,16 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TI-SOP-305\Documents\MIS\PROYECTO EVALUACION USUARIOS TES\MARK IV\media\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B307425B-0A64-425F-9BFB-1DB0EDF1358C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CE51EE8-05E0-4E37-9F5A-C07DD193D5E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Retroalimentación " sheetId="1" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Retroalimentación '!$A$1:$F$30</definedName>
   </definedNames>
@@ -56,9 +53,6 @@
     <t>PROCESO</t>
   </si>
   <si>
-    <t>Total de Evaluaciones</t>
-  </si>
-  <si>
     <t>Calificación Promedio</t>
   </si>
   <si>
@@ -87,6 +81,9 @@
   </si>
   <si>
     <t xml:space="preserve">OBSERVACIONES SINIESTRO: </t>
+  </si>
+  <si>
+    <t>Total de Evaluaciones del Mes Actual:</t>
   </si>
 </sst>
 </file>
@@ -419,34 +416,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
@@ -462,6 +438,11 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -488,6 +469,22 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -642,47 +639,6 @@
     <xdr:clientData fLocksWithSheet="0"/>
   </xdr:oneCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Formato de Evaluación"/>
-      <sheetName val="Data"/>
-      <sheetName val="Procesos"/>
-      <sheetName val="Por asesor"/>
-      <sheetName val="Dash"/>
-      <sheetName val="Retroalimentación "/>
-      <sheetName val="Planeación"/>
-      <sheetName val="Consulta evaluación"/>
-      <sheetName val="Ranking "/>
-      <sheetName val="Tendencias"/>
-      <sheetName val="Hoja2"/>
-      <sheetName val="Hoja1"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1">
-        <row r="1">
-          <cell r="A1" t="str">
-            <v>ñ</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -953,8 +909,8 @@
   </sheetPr>
   <dimension ref="A1:AH1000"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:F12"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -975,14 +931,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:34" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
       <c r="G1" s="1"/>
       <c r="H1" s="2">
         <v>1</v>
@@ -1056,73 +1012,73 @@
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="14"/>
-      <c r="C2" s="15"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="22"/>
       <c r="D2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="14"/>
-      <c r="F2" s="15"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="22"/>
       <c r="G2" s="1"/>
       <c r="H2" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="U2" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="V2" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="W2" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="X2" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="Y2" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="Z2" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="AA2" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="AB2" s="1"/>
       <c r="AC2" s="1"/>
@@ -1136,73 +1092,73 @@
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="14"/>
-      <c r="C3" s="15"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="22"/>
       <c r="D3" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
-      <c r="E3" s="14"/>
-      <c r="F3" s="15"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="22"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="T3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="U3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="V3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="W3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="X3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="Y3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="Z3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="AA3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="AB3" s="1"/>
       <c r="AC3" s="1"/>
@@ -1214,75 +1170,75 @@
     </row>
     <row r="4" spans="1:34" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="38"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="16"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="17"/>
-      <c r="F4" s="15"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="22"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="S4" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="T4" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="U4" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="V4" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="W4" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="X4" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="Y4" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="Z4" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="AA4" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="AB4" s="1"/>
       <c r="AC4" s="1"/>
@@ -1293,15 +1249,15 @@
       <c r="AH4" s="1"/>
     </row>
     <row r="5" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="30" t="s">
+      <c r="A5" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="22"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="15"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="30" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="15"/>
+      <c r="E5" s="22"/>
       <c r="F5" s="4"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
@@ -1333,14 +1289,14 @@
       <c r="AH5" s="1"/>
     </row>
     <row r="6" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
-        <v>14</v>
+      <c r="A6" s="23" t="s">
+        <v>13</v>
       </c>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
+      <c r="B6" s="24"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
@@ -1371,12 +1327,12 @@
       <c r="AH6" s="1"/>
     </row>
     <row r="7" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="31"/>
-      <c r="B7" s="32"/>
-      <c r="C7" s="32"/>
-      <c r="D7" s="32"/>
-      <c r="E7" s="32"/>
-      <c r="F7" s="33"/>
+      <c r="A7" s="25"/>
+      <c r="B7" s="26"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="27"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
@@ -1407,12 +1363,12 @@
       <c r="AH7" s="1"/>
     </row>
     <row r="8" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="34"/>
-      <c r="B8" s="35"/>
-      <c r="C8" s="35"/>
-      <c r="D8" s="35"/>
-      <c r="E8" s="35"/>
-      <c r="F8" s="36"/>
+      <c r="A8" s="28"/>
+      <c r="B8" s="29"/>
+      <c r="C8" s="29"/>
+      <c r="D8" s="29"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="30"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
@@ -1443,15 +1399,15 @@
       <c r="AH8" s="1"/>
     </row>
     <row r="9" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="34"/>
-      <c r="B9" s="35"/>
-      <c r="C9" s="35"/>
-      <c r="D9" s="35"/>
-      <c r="E9" s="35"/>
-      <c r="F9" s="36"/>
+      <c r="A9" s="28"/>
+      <c r="B9" s="29"/>
+      <c r="C9" s="29"/>
+      <c r="D9" s="29"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="30"/>
       <c r="G9" s="1"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="9"/>
+      <c r="H9" s="34"/>
+      <c r="I9" s="12"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
@@ -1479,15 +1435,15 @@
       <c r="AH9" s="1"/>
     </row>
     <row r="10" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="34"/>
-      <c r="B10" s="35"/>
-      <c r="C10" s="35"/>
-      <c r="D10" s="35"/>
-      <c r="E10" s="35"/>
-      <c r="F10" s="36"/>
+      <c r="A10" s="28"/>
+      <c r="B10" s="29"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="29"/>
+      <c r="F10" s="30"/>
       <c r="G10" s="1"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
@@ -1515,15 +1471,15 @@
       <c r="AH10" s="1"/>
     </row>
     <row r="11" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="34"/>
-      <c r="B11" s="35"/>
-      <c r="C11" s="35"/>
-      <c r="D11" s="35"/>
-      <c r="E11" s="35"/>
-      <c r="F11" s="36"/>
+      <c r="A11" s="28"/>
+      <c r="B11" s="29"/>
+      <c r="C11" s="29"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="29"/>
+      <c r="F11" s="30"/>
       <c r="G11" s="1"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
@@ -1551,15 +1507,15 @@
       <c r="AH11" s="1"/>
     </row>
     <row r="12" spans="1:34" ht="226.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="37"/>
-      <c r="B12" s="38"/>
-      <c r="C12" s="38"/>
-      <c r="D12" s="38"/>
-      <c r="E12" s="38"/>
-      <c r="F12" s="39"/>
+      <c r="A12" s="31"/>
+      <c r="B12" s="32"/>
+      <c r="C12" s="32"/>
+      <c r="D12" s="32"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="33"/>
       <c r="G12" s="1"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="9"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
@@ -1587,14 +1543,14 @@
       <c r="AH12" s="1"/>
     </row>
     <row r="13" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A13" s="10" t="s">
-        <v>8</v>
+      <c r="A13" s="23" t="s">
+        <v>7</v>
       </c>
-      <c r="B13" s="11"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
+      <c r="B13" s="24"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="24"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="24"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
@@ -1625,12 +1581,12 @@
       <c r="AH13" s="1"/>
     </row>
     <row r="14" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A14" s="18"/>
-      <c r="B14" s="19"/>
-      <c r="C14" s="19"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="19"/>
-      <c r="F14" s="20"/>
+      <c r="A14" s="8"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="10"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
@@ -1661,12 +1617,12 @@
       <c r="AH14" s="1"/>
     </row>
     <row r="15" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A15" s="21"/>
-      <c r="B15" s="9"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="22"/>
+      <c r="A15" s="11"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="13"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
@@ -1697,12 +1653,12 @@
       <c r="AH15" s="1"/>
     </row>
     <row r="16" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="21"/>
-      <c r="B16" s="9"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="22"/>
+      <c r="A16" s="11"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="13"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
@@ -1733,12 +1689,12 @@
       <c r="AH16" s="1"/>
     </row>
     <row r="17" spans="1:34" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="21"/>
-      <c r="B17" s="9"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="22"/>
+      <c r="A17" s="11"/>
+      <c r="B17" s="12"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="13"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
@@ -1769,12 +1725,12 @@
       <c r="AH17" s="1"/>
     </row>
     <row r="18" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="21"/>
-      <c r="B18" s="9"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="22"/>
+      <c r="A18" s="11"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="13"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
@@ -1805,12 +1761,12 @@
       <c r="AH18" s="1"/>
     </row>
     <row r="19" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="23"/>
-      <c r="B19" s="24"/>
-      <c r="C19" s="24"/>
-      <c r="D19" s="24"/>
-      <c r="E19" s="24"/>
-      <c r="F19" s="25"/>
+      <c r="A19" s="14"/>
+      <c r="B19" s="15"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="16"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
@@ -1878,11 +1834,11 @@
     </row>
     <row r="21" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
-      <c r="B21" s="26"/>
-      <c r="C21" s="24"/>
-      <c r="D21" s="24"/>
-      <c r="E21" s="24"/>
-      <c r="F21" s="24"/>
+      <c r="B21" s="17"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="15"/>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
@@ -1914,15 +1870,15 @@
     </row>
     <row r="22" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="B22" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="C22" s="28"/>
-      <c r="D22" s="28"/>
-      <c r="E22" s="28"/>
-      <c r="F22" s="29"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="19"/>
+      <c r="E22" s="19"/>
+      <c r="F22" s="20"/>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
@@ -2098,7 +2054,7 @@
     </row>
     <row r="27" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -2208,7 +2164,7 @@
     </row>
     <row r="30" spans="1:34" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B30" s="1"/>
       <c r="C30" s="7"/>
@@ -10216,13 +10172,6 @@
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A14:F19"/>
-    <mergeCell ref="B21:F21"/>
-    <mergeCell ref="B22:F22"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="A6:F6"/>
-    <mergeCell ref="A7:F12"/>
     <mergeCell ref="H9:I12"/>
     <mergeCell ref="A13:F13"/>
     <mergeCell ref="A1:F1"/>
@@ -10232,6 +10181,13 @@
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="E4:F4"/>
+    <mergeCell ref="A14:F19"/>
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="B22:F22"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="A7:F12"/>
   </mergeCells>
   <conditionalFormatting sqref="B20 B23:B37">
     <cfRule type="beginsWith" dxfId="6" priority="3" operator="beginsWith" text="N">

</xml_diff>